<commit_message>
switch to tau from mu
</commit_message>
<xml_diff>
--- a/data/physiology/BremerDennis_EcoSalPlus_2008.xlsx
+++ b/data/physiology/BremerDennis_EcoSalPlus_2008.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flamholz/Documents/workspace/redox-proteome/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flamholz/Documents/workspace/redox-proteome/data/physiology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4872FBE5-DE0C-1949-B974-DB8D4018EFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D21CFA3-442B-F149-9D16-EA5B53A9EEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{E4CCB114-1991-EC42-8D48-ED12DEA40969}"/>
+    <workbookView xWindow="-34680" yWindow="340" windowWidth="27640" windowHeight="16440" xr2:uid="{E4CCB114-1991-EC42-8D48-ED12DEA40969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -1140,22 +1140,22 @@
     <t>observed_parameters</t>
   </si>
   <si>
-    <t>u_0.6</t>
-  </si>
-  <si>
-    <t>u_1.0</t>
-  </si>
-  <si>
-    <t>u_1.5</t>
-  </si>
-  <si>
-    <t>u_2.0</t>
-  </si>
-  <si>
-    <t>u_3.0</t>
-  </si>
-  <si>
-    <t>u_2.5</t>
+    <t>t_100_min</t>
+  </si>
+  <si>
+    <t>t_60_min</t>
+  </si>
+  <si>
+    <t>t_40_min</t>
+  </si>
+  <si>
+    <t>t_30_min</t>
+  </si>
+  <si>
+    <t>t_24_min</t>
+  </si>
+  <si>
+    <t>t_20_min</t>
   </si>
 </sst>
 </file>
@@ -1539,7 +1539,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1571,10 +1571,10 @@
         <v>75</v>
       </c>
       <c r="H1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" t="s">
         <v>77</v>
-      </c>
-      <c r="I1" t="s">
-        <v>76</v>
       </c>
       <c r="J1" t="s">
         <v>71</v>

</xml_diff>